<commit_message>
#85: Confirms output stability and builds proper conversion from Excel to PDF
</commit_message>
<xml_diff>
--- a/paper_slides/code/latex_test_widetable.xlsx
+++ b/paper_slides/code/latex_test_widetable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sameernair-desai/Desktop/InstRes/SIEPR_RA/template/paper_slides/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA9C63E3-F5E6-914A-BBF0-77F8A287474A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF023910-6C53-8048-BB4D-2B68C1C8C0EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32900" yWindow="2600" windowWidth="34360" windowHeight="17440" activeTab="1" xr2:uid="{B390F614-ADA4-ED45-B7F9-CAB4E813F00D}"/>
+    <workbookView xWindow="38080" yWindow="3020" windowWidth="34360" windowHeight="17440" activeTab="1" xr2:uid="{B390F614-ADA4-ED45-B7F9-CAB4E813F00D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,40 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
-  <si>
-    <t>Strong</t>
-  </si>
-  <si>
-    <t>Democrat</t>
-  </si>
-  <si>
-    <t>Independent</t>
-  </si>
-  <si>
-    <t>Republican</t>
-  </si>
-  <si>
-    <t>Seen Banner</t>
-  </si>
-  <si>
-    <t>Table S2: Experimental Summary Statistics by Political Leaning</t>
-  </si>
-  <si>
-    <t>Clicked Banner</t>
-  </si>
-  <si>
-    <t>Consented</t>
-  </si>
-  <si>
-    <t>Completed Baseline Survey</t>
-  </si>
-  <si>
-    <t>Completed Endline Survey</t>
-  </si>
-  <si>
-    <t>Total Attrition Rate</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="14">
   <si>
     <r>
       <rPr>
@@ -93,6 +60,45 @@
       </rPr>
       <t>Based on 𝛽 = 0.932 coefficient of stability.</t>
     </r>
+  </si>
+  <si>
+    <t>Group 1</t>
+  </si>
+  <si>
+    <t>Group 2</t>
+  </si>
+  <si>
+    <t>Group 3</t>
+  </si>
+  <si>
+    <t>Group 4</t>
+  </si>
+  <si>
+    <t>Group 5</t>
+  </si>
+  <si>
+    <t>###</t>
+  </si>
+  <si>
+    <t>Condition 1</t>
+  </si>
+  <si>
+    <t>Condition 5</t>
+  </si>
+  <si>
+    <t>Condition 6</t>
+  </si>
+  <si>
+    <t>Condition 4</t>
+  </si>
+  <si>
+    <t>Condition 3</t>
+  </si>
+  <si>
+    <t>Condition 2</t>
+  </si>
+  <si>
+    <t>Table S2: Experimental Summary Statistics by Group and Condition</t>
   </si>
 </sst>
 </file>
@@ -182,7 +188,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -208,6 +214,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,32 +530,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D491D851-0BDE-2243-9EB9-D84ECB9E783F}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F12"/>
+      <selection activeCell="A5" sqref="A5:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="11"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -556,184 +564,155 @@
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
-      <c r="B4" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
-      <c r="F4" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6">
-        <v>3436123</v>
-      </c>
-      <c r="C5" s="6">
-        <v>5245121</v>
-      </c>
-      <c r="D5" s="6">
-        <v>850321</v>
-      </c>
-      <c r="E5" s="6">
-        <v>3506722</v>
-      </c>
-      <c r="F5" s="6">
-        <v>1519232</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="6">
-        <f>B5*0.85</f>
-        <v>2920704.55</v>
-      </c>
-      <c r="C6" s="6">
-        <f t="shared" ref="C6:F6" si="0">C5*0.85</f>
-        <v>4458352.8499999996</v>
-      </c>
-      <c r="D6" s="6">
-        <f t="shared" si="0"/>
-        <v>722772.85</v>
-      </c>
-      <c r="E6" s="6">
-        <f t="shared" si="0"/>
-        <v>2980713.6999999997</v>
-      </c>
-      <c r="F6" s="6">
-        <f t="shared" si="0"/>
-        <v>1291347.2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="6">
-        <f>0.23*B6</f>
-        <v>671762.04649999994</v>
-      </c>
-      <c r="C7" s="6">
-        <f t="shared" ref="C7:F7" si="1">0.23*C6</f>
-        <v>1025421.1555</v>
-      </c>
-      <c r="D7" s="6">
-        <f t="shared" si="1"/>
-        <v>166237.7555</v>
-      </c>
-      <c r="E7" s="6">
-        <f t="shared" si="1"/>
-        <v>685564.15099999995</v>
-      </c>
-      <c r="F7" s="6">
-        <f t="shared" si="1"/>
-        <v>297009.85600000003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="6">
-        <f>0.45*B7</f>
-        <v>302292.92092499998</v>
-      </c>
-      <c r="C8" s="6">
-        <f t="shared" ref="C8:F8" si="2">0.45*C7</f>
-        <v>461439.519975</v>
-      </c>
-      <c r="D8" s="6">
-        <f t="shared" si="2"/>
-        <v>74806.989975000004</v>
-      </c>
-      <c r="E8" s="6">
-        <f t="shared" si="2"/>
-        <v>308503.86794999999</v>
-      </c>
-      <c r="F8" s="6">
-        <f t="shared" si="2"/>
-        <v>133654.43520000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="7">
-        <f>0.12*B8</f>
-        <v>36275.150511</v>
-      </c>
-      <c r="C9" s="7">
-        <f t="shared" ref="C9:F9" si="3">0.12*C8</f>
-        <v>55372.742397000002</v>
-      </c>
-      <c r="D9" s="7">
-        <f t="shared" si="3"/>
-        <v>8976.8387970000003</v>
-      </c>
-      <c r="E9" s="7">
-        <f t="shared" si="3"/>
-        <v>37020.464153999994</v>
-      </c>
-      <c r="F9" s="7">
-        <f t="shared" si="3"/>
-        <v>16038.532224</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="8">
-        <f>(B5-B9)/B5</f>
-        <v>0.98944300000000007</v>
-      </c>
-      <c r="C10" s="8">
-        <f t="shared" ref="C10:F10" si="4">(C5-C9)/C5</f>
-        <v>0.98944299999999996</v>
-      </c>
-      <c r="D10" s="8">
-        <f t="shared" si="4"/>
-        <v>0.98944299999999996</v>
-      </c>
-      <c r="E10" s="8">
-        <f t="shared" si="4"/>
-        <v>0.98944300000000007</v>
-      </c>
-      <c r="F10" s="8">
-        <f t="shared" si="4"/>
-        <v>0.98944300000000007</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -742,6 +721,7 @@
     <mergeCell ref="A2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -750,14 +730,20 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -776,36 +762,32 @@
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
-      <c r="B4" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
-      <c r="F4" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B5" s="6">
         <v>3436123</v>
@@ -825,7 +807,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B6" s="6">
         <f>B5*0.85</f>
@@ -850,7 +832,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B7" s="6">
         <f>0.23*B6</f>
@@ -875,7 +857,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B8" s="6">
         <f>0.45*B7</f>
@@ -899,8 +881,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>9</v>
+      <c r="A9" t="s">
+        <v>8</v>
       </c>
       <c r="B9" s="7">
         <f>0.12*B8</f>
@@ -925,7 +907,7 @@
     </row>
     <row r="10" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="8">
         <f>(B5-B9)/B5</f>
@@ -950,7 +932,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -959,5 +941,6 @@
     <mergeCell ref="A2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>